<commit_message>
[IMP] z0bug_odoo: new configuration
</commit_message>
<xml_diff>
--- a/z0bug_odoo/build/lib.linux-x86_64-2.7/z0bug_odoo/data/account_invoice_line.xlsx
+++ b/z0bug_odoo/build/lib.linux-x86_64-2.7/z0bug_odoo/data/account_invoice_line.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="220">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t xml:space="preserve">z0bug.tax_a41v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.invoice_Z0_4_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prodotto Zeta (versione EU)</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.invoice_Z0_5_1</t>
@@ -684,7 +690,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -725,6 +731,11 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -776,7 +787,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -805,6 +816,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,12 +837,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1861,73 +1876,70 @@
         <v>154</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>156</v>
+        <v>132</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>103</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>18</v>
+        <v>1.5</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>161</v>
+      <c r="H37" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J37" s="1"/>
-      <c r="L37" s="6" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="F38" s="1" t="n">
         <v>100</v>
@@ -1936,35 +1948,38 @@
         <v>103</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="J38" s="1"/>
+      <c r="L38" s="7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>103</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>20</v>
@@ -1976,23 +1991,23 @@
         <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>20</v>
@@ -2004,14 +2019,14 @@
         <v>170</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>150</v>
@@ -2020,7 +2035,7 @@
         <v>34</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>20</v>
@@ -2029,26 +2044,26 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>172</v>
+        <v>58</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>20</v>
@@ -2057,143 +2072,143 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H43" s="1" t="n">
-        <v>1500</v>
+        <v>34</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>179</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="J43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H44" s="1" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J44" s="1"/>
+        <v>180</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>33</v>
+        <v>184</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>143</v>
+        <v>185</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="J45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>190</v>
+        <v>33</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H46" s="1" t="n">
-        <v>0.475</v>
+        <v>188</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="J46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>20</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H47" s="1" t="n">
         <v>0.475</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J47" s="1"/>
     </row>
@@ -2202,26 +2217,26 @@
         <v>193</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F48" s="1" t="n">
         <v>20</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>-0.475</v>
+        <v>0.475</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J48" s="1"/>
     </row>
@@ -2230,195 +2245,223 @@
         <v>195</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>-0.475</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="J50" s="1"/>
-      <c r="K50" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M50" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N50" s="4" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N51" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="F51" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F52" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H52" s="1" t="n">
-        <v>60</v>
+        <v>188</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>178</v>
+        <v>208</v>
       </c>
       <c r="J52" s="1"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="N52" s="2" t="s">
-        <v>211</v>
-      </c>
+      <c r="K52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="F53" s="1" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="J53" s="1"/>
-      <c r="K53" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>215</v>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F54" s="1" t="n">
+      <c r="E55" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F55" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H54" s="1" t="s">
+      <c r="G55" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I54" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
+      <c r="I55" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>